<commit_message>
update for the forth analysis (including more modes)
</commit_message>
<xml_diff>
--- a/选择竖弯模态.xlsx
+++ b/选择竖弯模态.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\xihoumen_inverse_force_estimation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\xihoumen_inverse_force_estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC78C504-CE03-4821-A682-9E50849BE3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BA7C9A-FA30-463C-99A6-267D04C8746A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28815" yWindow="240" windowWidth="9450" windowHeight="20505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57465" yWindow="2550" windowWidth="28650" windowHeight="15105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$151</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -365,15 +368,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>2</v>
       </c>
@@ -381,7 +385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -389,7 +393,7 @@
         <v>5.44419405273101E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -400,7 +404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -411,7 +415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -419,7 +423,7 @@
         <v>0.120810281799328</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -430,7 +434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -444,7 +448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -455,7 +459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -463,7 +467,7 @@
         <v>0.18940295395762299</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -471,7 +475,7 @@
         <v>0.19566052005397799</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -479,7 +483,7 @@
         <v>0.204095551423886</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -487,7 +491,7 @@
         <v>0.213198659482907</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -495,7 +499,7 @@
         <v>0.21572840205846</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -506,7 +510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -514,7 +518,7 @@
         <v>0.23388125123783299</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -522,7 +526,7 @@
         <v>0.234860864461336</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -530,7 +534,7 @@
         <v>0.23905068054397899</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -538,7 +542,7 @@
         <v>0.24418229042932299</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -546,7 +550,7 @@
         <v>0.25361445427249402</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -554,7 +558,7 @@
         <v>0.25831852363339403</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -565,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -573,7 +577,7 @@
         <v>0.32028241903641302</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -584,7 +588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -592,7 +596,7 @@
         <v>0.34092789847188798</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -600,7 +604,7 @@
         <v>0.34157899410285197</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -608,7 +612,7 @@
         <v>0.34984096195127301</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -616,7 +620,7 @@
         <v>0.35724661760106802</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -630,7 +634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -638,7 +642,7 @@
         <v>0.37493843280892197</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -646,7 +650,7 @@
         <v>0.38501258969043201</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -654,7 +658,7 @@
         <v>0.38813277736787499</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -662,7 +666,7 @@
         <v>0.39659495069505202</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -670,7 +674,7 @@
         <v>0.39737822530442801</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -681,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -689,7 +693,7 @@
         <v>0.42994198745513101</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -697,7 +701,7 @@
         <v>0.44604398138879903</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -705,7 +709,7 @@
         <v>0.45662340350883102</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -713,7 +717,7 @@
         <v>0.45949139053778099</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -721,7 +725,7 @@
         <v>0.47024617837241001</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -732,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -740,7 +744,7 @@
         <v>0.48033179728541697</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -748,7 +752,7 @@
         <v>0.51021076773030505</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -756,7 +760,7 @@
         <v>0.51615755404957597</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -767,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -778,7 +782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -786,7 +790,7 @@
         <v>0.55214587516793101</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -797,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -805,7 +809,7 @@
         <v>0.58829225933919205</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -813,7 +817,7 @@
         <v>0.59081864173075804</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -824,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -832,7 +836,7 @@
         <v>0.59861496752800503</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -840,7 +844,7 @@
         <v>0.64365498804909804</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -851,7 +855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -859,7 +863,7 @@
         <v>0.66115266782024396</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -867,7 +871,7 @@
         <v>0.66553210343973301</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -875,7 +879,7 @@
         <v>0.66563137983197096</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -883,7 +887,7 @@
         <v>0.67890079706504403</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -891,7 +895,7 @@
         <v>0.679344566046584</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -899,7 +903,7 @@
         <v>0.69001921219181594</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -910,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -918,7 +922,7 @@
         <v>0.72632413415749797</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -929,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -937,7 +941,7 @@
         <v>0.74500410301715003</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -945,7 +949,7 @@
         <v>0.74615304010144201</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -953,7 +957,7 @@
         <v>0.79130470796591801</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -964,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -972,7 +976,7 @@
         <v>0.82330353720941996</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -980,7 +984,7 @@
         <v>0.82442960808523702</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -988,7 +992,7 @@
         <v>0.84078258174032405</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -999,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1007,7 +1011,7 @@
         <v>0.87137555834333102</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1018,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1026,7 +1030,7 @@
         <v>0.90120488703804802</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1034,7 +1038,7 @@
         <v>0.901720465091848</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1042,7 +1046,7 @@
         <v>0.90308354046077399</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1050,7 +1054,7 @@
         <v>0.90325144797275203</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1061,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1069,7 +1073,7 @@
         <v>0.93882413189314196</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1080,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1088,7 +1092,7 @@
         <v>0.98265870529966604</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1096,7 +1100,7 @@
         <v>0.98320716653349405</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1104,7 +1108,7 @@
         <v>0.99039773875803905</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1112,7 +1116,7 @@
         <v>1.0111734619117401</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1123,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1131,7 +1135,7 @@
         <v>1.0629523351393999</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1139,7 +1143,7 @@
         <v>1.06395486982064</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1147,7 +1151,7 @@
         <v>1.0841895405074</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1158,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1166,7 +1170,7 @@
         <v>1.0955547459629</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>1.1246791614568601</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -1182,7 +1186,7 @@
         <v>1.12842869523306</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -1190,7 +1194,7 @@
         <v>1.14322062004493</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -1198,7 +1202,7 @@
         <v>1.1450216525155501</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -1206,7 +1210,7 @@
         <v>1.1456042335451899</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -1217,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -1225,7 +1229,7 @@
         <v>1.1953476399635801</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -1233,7 +1237,7 @@
         <v>1.2231965795977999</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -1241,7 +1245,7 @@
         <v>1.22663775087822</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -1252,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -1260,7 +1264,7 @@
         <v>1.26056696269413</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -1268,7 +1272,7 @@
         <v>1.27281184363695</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -1276,7 +1280,7 @@
         <v>1.2987691075103001</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -1284,7 +1288,7 @@
         <v>1.30116125518031</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -1292,7 +1296,7 @@
         <v>1.3086677258764501</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -1300,7 +1304,7 @@
         <v>1.3297137595106701</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -1308,7 +1312,7 @@
         <v>1.34038930751023</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -1316,7 +1320,7 @@
         <v>1.3551251393372601</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -1324,7 +1328,7 @@
         <v>1.3598621693539501</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -1332,7 +1336,7 @@
         <v>1.3729845496303299</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -1340,7 +1344,7 @@
         <v>1.3805211459881299</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -1348,7 +1352,7 @@
         <v>1.3911885112039899</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -1356,7 +1360,7 @@
         <v>1.4200353113998601</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -1364,7 +1368,7 @@
         <v>1.42535517497631</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -1372,7 +1376,7 @@
         <v>1.4311920673268299</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -1380,7 +1384,7 @@
         <v>1.44646261237801</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -1388,7 +1392,7 @@
         <v>1.4533751087162601</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -1396,7 +1400,7 @@
         <v>1.4557814516657901</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -1404,7 +1408,7 @@
         <v>1.47416761396638</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -1412,7 +1416,7 @@
         <v>1.4911261578519699</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -1420,7 +1424,7 @@
         <v>1.53404114219973</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -1428,7 +1432,7 @@
         <v>1.5376686550415</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -1436,7 +1440,7 @@
         <v>1.5576395112852099</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -1444,7 +1448,7 @@
         <v>1.5644679773013099</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -1452,7 +1456,7 @@
         <v>1.58372745913596</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -1460,7 +1464,7 @@
         <v>1.59036171013112</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -1468,7 +1472,7 @@
         <v>1.5968297092835899</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -1476,7 +1480,7 @@
         <v>1.60606201700966</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -1484,7 +1488,7 @@
         <v>1.61081656152282</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -1492,7 +1496,7 @@
         <v>1.6416059064208099</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -1500,7 +1504,7 @@
         <v>1.6471675974801101</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -1508,7 +1512,7 @@
         <v>1.66361451613171</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -1516,7 +1520,7 @@
         <v>1.6941148086459901</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -1524,7 +1528,7 @@
         <v>1.72608977151095</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -1532,7 +1536,7 @@
         <v>1.72996910003131</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -1540,7 +1544,7 @@
         <v>1.7666467207408301</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -1548,7 +1552,7 @@
         <v>1.77813832861761</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -1556,7 +1560,7 @@
         <v>1.7943558097260199</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -1564,7 +1568,7 @@
         <v>1.81110468384196</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -1572,7 +1576,7 @@
         <v>1.81402434775465</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -1580,7 +1584,7 @@
         <v>1.83998508971481</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -1588,7 +1592,7 @@
         <v>1.84140556636998</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -1596,7 +1600,7 @@
         <v>1.8447003667447499</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -1604,7 +1608,7 @@
         <v>1.8562562911495299</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -1612,7 +1616,7 @@
         <v>1.8603616107710399</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -1620,7 +1624,7 @@
         <v>1.8740554513804299</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -1628,7 +1632,7 @@
         <v>1.8766632358215201</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -1636,7 +1640,7 @@
         <v>1.8893692116797001</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -1644,7 +1648,7 @@
         <v>1.8936707606581999</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -1652,7 +1656,7 @@
         <v>1.89667165513198</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -1660,7 +1664,7 @@
         <v>1.8994199876984399</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -1669,6 +1673,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C151" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
udpate for plot a figure in excel
</commit_message>
<xml_diff>
--- a/选择竖弯模态.xlsx
+++ b/选择竖弯模态.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\xihoumen_inverse_force_estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BA7C9A-FA30-463C-99A6-267D04C8746A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942CCC80-7F09-4566-88EE-98EDB97A9B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57465" yWindow="2550" windowWidth="28650" windowHeight="15105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28785" yWindow="2550" windowWidth="28650" windowHeight="15105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$151</definedName>
@@ -103,6 +104,1092 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Modes whose frequencies are</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t> under 1.2Hz</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-FD2B-4B0C-AAF0-9492A7A7065C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-FD2B-4B0C-AAF0-9492A7A7065C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-FD2B-4B0C-AAF0-9492A7A7065C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>9.3670906483855704E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.101787518996202</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13203300929921299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17792338772373301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17953587902354301</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22738865906689101</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27189473709811401</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.321444530999279</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.37095473595174999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.42380329730566901</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.476438033179025</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.52347215327470598</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.54760715014832695</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.58751705916205499</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.59577666179543698</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.64615338206993</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.69168507607792595</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.73883766019361896</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.79254281004715399</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.84746360751871996</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.90070657161735801</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.91253619796553898</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.96506389083276201</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0260245654584801</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.08947280237691</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.1584985609426699</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.2293508930892101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FD2B-4B0C-AAF0-9492A7A7065C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="32273424"/>
+        <c:axId val="32271504"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="32273424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="32271504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="32271504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="32273424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>399096</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4ED25EB-6CE5-0CE7-5512-8777AA218531}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,8 +1458,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1683,4 +2770,237 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBAE868-C3C8-46D4-BB72-5B81A7E2E690}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>9.3670906483855704E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0.101787518996202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.13203300929921299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.17792338772373301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.17953587902354301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>0.22738865906689101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>0.27189473709811401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>0.321444530999279</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>0.37095473595174999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>0.42380329730566901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>0.476438033179025</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <v>0.52347215327470598</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>44</v>
+      </c>
+      <c r="B13">
+        <v>0.54760715014832695</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <v>0.58751705916205499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>49</v>
+      </c>
+      <c r="B15">
+        <v>0.59577666179543698</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>52</v>
+      </c>
+      <c r="B16">
+        <v>0.64615338206993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>59</v>
+      </c>
+      <c r="B17">
+        <v>0.69168507607792595</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>61</v>
+      </c>
+      <c r="B18">
+        <v>0.73883766019361896</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>65</v>
+      </c>
+      <c r="B19">
+        <v>0.79254281004715399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>69</v>
+      </c>
+      <c r="B20">
+        <v>0.84746360751871996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>71</v>
+      </c>
+      <c r="B21">
+        <v>0.90070657161735801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>76</v>
+      </c>
+      <c r="B22">
+        <v>0.91253619796553898</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>78</v>
+      </c>
+      <c r="B23">
+        <v>0.96506389083276201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>83</v>
+      </c>
+      <c r="B24">
+        <v>1.0260245654584801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>87</v>
+      </c>
+      <c r="B25">
+        <v>1.08947280237691</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>94</v>
+      </c>
+      <c r="B26">
+        <v>1.1584985609426699</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>98</v>
+      </c>
+      <c r="B27">
+        <v>1.2293508930892101</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>